<commit_message>
memperbaiki file yang corupt dan merge kembali
</commit_message>
<xml_diff>
--- a/BurndownChart Signal grup.xlsx
+++ b/BurndownChart Signal grup.xlsx
@@ -522,7 +522,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>6</c:v>
@@ -553,11 +553,11 @@
           <c:showVal val="1"/>
         </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="66405888"/>
-        <c:axId val="66407424"/>
+        <c:axId val="91016192"/>
+        <c:axId val="92267264"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="66405888"/>
+        <c:axId val="91016192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -598,14 +598,14 @@
             <a:endParaRPr lang="id-ID"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="66407424"/>
+        <c:crossAx val="92267264"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="66407424"/>
+        <c:axId val="92267264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -654,7 +654,7 @@
             <a:endParaRPr lang="id-ID"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="66405888"/>
+        <c:crossAx val="91016192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -727,7 +727,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1025,7 +1025,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1036,7 +1036,7 @@
   <dimension ref="A1:S71"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E1" sqref="A1:XFD1"/>
+      <selection activeCell="C9" activeCellId="1" sqref="K48 C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1066,7 +1066,7 @@
         <v>6</v>
       </c>
       <c r="E3" s="4">
-        <f t="shared" ref="E3:F3" si="0">+F3+1</f>
+        <f t="shared" ref="E3" si="0">+F3+1</f>
         <v>41809</v>
       </c>
       <c r="F3" s="4">
@@ -1074,7 +1074,7 @@
         <v>41808</v>
       </c>
       <c r="G3" s="4">
-        <f t="shared" ref="G3:Q3" si="1">+H3+1</f>
+        <f t="shared" ref="G3:P3" si="1">+H3+1</f>
         <v>41807</v>
       </c>
       <c r="H3" s="4">
@@ -1260,7 +1260,7 @@
         <v>0</v>
       </c>
       <c r="K6" s="7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L6" s="7">
         <v>1</v>
@@ -1838,7 +1838,7 @@
         <v>0</v>
       </c>
       <c r="K17" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L17" s="7">
         <v>2</v>
@@ -2007,7 +2007,7 @@
       </c>
       <c r="K21" s="7">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="L21" s="7">
         <f t="shared" si="4"/>

</xml_diff>

<commit_message>
fix edit stylus dan text
</commit_message>
<xml_diff>
--- a/BurndownChart Signal grup.xlsx
+++ b/BurndownChart Signal grup.xlsx
@@ -510,19 +510,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>6</c:v>
@@ -553,11 +553,11 @@
           <c:showVal val="1"/>
         </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="91016192"/>
-        <c:axId val="92267264"/>
+        <c:axId val="53988352"/>
+        <c:axId val="53998336"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="91016192"/>
+        <c:axId val="53988352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -598,14 +598,14 @@
             <a:endParaRPr lang="id-ID"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="92267264"/>
+        <c:crossAx val="53998336"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="92267264"/>
+        <c:axId val="53998336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -654,7 +654,7 @@
             <a:endParaRPr lang="id-ID"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="91016192"/>
+        <c:crossAx val="53988352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -727,7 +727,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1025,7 +1025,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1036,7 +1036,7 @@
   <dimension ref="A1:S71"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C9" activeCellId="1" sqref="K48 C9"/>
+      <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1412,7 +1412,7 @@
         <v>0</v>
       </c>
       <c r="I9" s="7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J9" s="7">
         <v>0</v>
@@ -1458,7 +1458,7 @@
         <v>0</v>
       </c>
       <c r="G10" s="7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H10" s="7">
         <v>0</v>
@@ -1522,7 +1522,7 @@
         <v>0</v>
       </c>
       <c r="K11" s="7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L11" s="7">
         <v>0</v>
@@ -1667,7 +1667,7 @@
         <v>0</v>
       </c>
       <c r="F14" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G14" s="7">
         <v>0</v>
@@ -1770,13 +1770,13 @@
         <v>12</v>
       </c>
       <c r="E16" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F16" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G16" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H16" s="7">
         <v>0</v>
@@ -1784,7 +1784,9 @@
       <c r="I16" s="7">
         <v>0</v>
       </c>
-      <c r="J16" s="7"/>
+      <c r="J16" s="7">
+        <v>0</v>
+      </c>
       <c r="K16" s="7">
         <v>0</v>
       </c>
@@ -1820,19 +1822,19 @@
         <v>12</v>
       </c>
       <c r="E17" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F17" s="7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G17" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H17" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I17" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J17" s="7">
         <v>0</v>
@@ -1983,23 +1985,23 @@
       </c>
       <c r="E21" s="7">
         <f t="shared" ref="E21:P21" si="4">SUM(E4:E17)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F21" s="7">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G21" s="7">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H21" s="7">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I21" s="7">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J21" s="7">
         <f t="shared" si="4"/>
@@ -2007,7 +2009,7 @@
       </c>
       <c r="K21" s="7">
         <f t="shared" si="4"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="L21" s="7">
         <f t="shared" si="4"/>

</xml_diff>